<commit_message>
updates for new project facet
</commit_message>
<xml_diff>
--- a/data/cci/cci-schemes.xlsx
+++ b/data/cci/cci-schemes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies/data/cci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BED23B-A711-6048-8D1F-4A4DB0A3AEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233C7F3E-51AF-644E-88AD-E27C404E7F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-71620" yWindow="-2440" windowWidth="30240" windowHeight="18880" xr2:uid="{B107F907-321D-DF43-80B1-3451B0C1D4B4}"/>
   </bookViews>
@@ -79,249 +79,6 @@
     <t>This concept scheme represents the ECVs used by the CCI project</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">&lt;p&gt;The CCI concept schemes are used to define concepts within an element of a Directory Reference Scheme. There are currently eight concept schemes defined: &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../dataType&gt;data type&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t>=..//ecv&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>ecv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t>=../scheme/cci/freq&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>frequency</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t>=../org&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>institutes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../platform&gt;platforms&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../procLev&gt;processing levels&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../product&gt;products&lt;/a&gt;, and &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../sensor&gt;sensors&lt;/a&gt;. The use of a concept scheme allows easy navigation up and down the tree.&lt;/p&gt;&lt;h5&gt;SKOS Navigation Down the Concept Scheme&lt;/h5&gt;&lt;img </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=conceptSchemeDown.svg /&gt;&lt;h5&gt;SKOS Navigation Up the Concept Scheme&lt;/h5&gt;&lt;img </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=conceptSchemeUp.svg /&gt;&lt;p&gt;As well as being concepts the the concepts are also named individuals of the &lt;a href=../../../ontology/cci&gt;CCI Ontology&lt;/a&gt; classes.&lt;h5&gt;OWL Classes&lt;/h5&gt;&lt;img </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t>=classes.svg /&gt;&lt;p&gt;&lt;/p&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>0.0.1</t>
   </si>
   <si>
@@ -446,6 +203,9 @@
   </si>
   <si>
     <t>This concept scheme represents the projects used by the CCI project</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The CCI concept schemes are used to define concepts within an element of a Directory Reference Scheme. There are currently eight concept schemes defined: &lt;a href=../dataType&gt;data type&lt;/a&gt;, &lt;a href=..//ecv&gt;ecv&lt;/a&gt;, &lt;a href=../scheme/cci/freq&gt;frequency&lt;/a&gt;, &lt;a href=../org&gt;institutes&lt;/a&gt;, &lt;a href=../platform&gt;platforms&lt;/a&gt;, &lt;a href=../platformGrp&gt;platform groups&lt;/a&gt;, &lt;a href=../platformProg&gt;platform programs&lt;/a&gt;, &lt;a href=../procLev&gt;processing levels&lt;/a&gt;, &lt;a href=../product&gt;products&lt;/a&gt;, &lt;a href=../project&gt;projects&lt;/a&gt;, and &lt;a href=../sensor&gt;sensors&lt;/a&gt;. The use of a concept scheme allows easy navigation up and down the tree.&lt;/p&gt;&lt;h5&gt;SKOS Navigation Down the Concept Scheme&lt;/h5&gt;&lt;img src=conceptSchemeDown.svg /&gt;&lt;h5&gt;SKOS Navigation Up the Concept Scheme&lt;/h5&gt;&lt;img src=conceptSchemeUp.svg /&gt;&lt;p&gt;As well as being concepts the the concepts are also named individuals of the &lt;a href=../../../ontology/cci&gt;CCI Ontology&lt;/a&gt; classes.&lt;h5&gt;OWL Classes&lt;/h5&gt;&lt;img src=classes.svg /&gt;&lt;p&gt;&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -455,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -486,12 +246,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Liberation Sans1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF313739"/>
-      <name val="Monospace"/>
     </font>
     <font>
       <sz val="10"/>
@@ -590,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -933,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF3300C-39A4-7B44-84E0-196A8940B2E9}">
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -2005,7 +1759,7 @@
       <c r="AMF1" s="4"/>
       <c r="AMG1" s="4"/>
     </row>
-    <row r="2" spans="1:1021" ht="70">
+    <row r="2" spans="1:1021" ht="84">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2028,29 +1782,29 @@
         <v>18</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:1021" ht="84">
+      <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:1021" ht="70">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -2059,32 +1813,32 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="4" spans="1:1021" ht="70">
+    <row r="4" spans="1:1021" ht="84">
       <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -2093,34 +1847,34 @@
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="5" spans="1:1021" ht="70">
+    <row r="5" spans="1:1021" ht="84">
       <c r="A5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -2129,32 +1883,32 @@
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="6" spans="1:1021" ht="70">
+    <row r="6" spans="1:1021" ht="84">
       <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -2163,32 +1917,32 @@
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="7" spans="1:1021" ht="70">
+    <row r="7" spans="1:1021" ht="84">
       <c r="A7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -2197,32 +1951,32 @@
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="8" spans="1:1021" ht="70">
+    <row r="8" spans="1:1021" ht="84">
       <c r="A8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -2231,32 +1985,32 @@
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="9" spans="1:1021" ht="70">
+    <row r="9" spans="1:1021" ht="84">
       <c r="A9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -2265,32 +2019,32 @@
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="10" spans="1:1021" ht="70">
+    <row r="10" spans="1:1021" ht="84">
       <c r="A10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2299,32 +2053,32 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="11" spans="1:1021" ht="70">
+    <row r="11" spans="1:1021" ht="84">
       <c r="A11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2333,32 +2087,32 @@
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="12" spans="1:1021" ht="70">
+    <row r="12" spans="1:1021" ht="84">
       <c r="A12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2367,20 +2121,20 @@
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update description fields in `cci-schemes.xlsx`
</commit_message>
<xml_diff>
--- a/data/cci/cci-schemes.xlsx
+++ b/data/cci/cci-schemes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies/data/cci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233C7F3E-51AF-644E-88AD-E27C404E7F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457DD7F1-6A72-AF4A-A9A6-956CAE4A9DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-71620" yWindow="-2440" windowWidth="30240" windowHeight="18880" xr2:uid="{B107F907-321D-DF43-80B1-3451B0C1D4B4}"/>
+    <workbookView xWindow="-32800" yWindow="-1580" windowWidth="30240" windowHeight="18880" xr2:uid="{B107F907-321D-DF43-80B1-3451B0C1D4B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
     <t>This concept scheme represents the projects used by the CCI project</t>
   </si>
   <si>
-    <t>&lt;p&gt;The CCI concept schemes are used to define concepts within an element of a Directory Reference Scheme. There are currently eight concept schemes defined: &lt;a href=../dataType&gt;data type&lt;/a&gt;, &lt;a href=..//ecv&gt;ecv&lt;/a&gt;, &lt;a href=../scheme/cci/freq&gt;frequency&lt;/a&gt;, &lt;a href=../org&gt;institutes&lt;/a&gt;, &lt;a href=../platform&gt;platforms&lt;/a&gt;, &lt;a href=../platformGrp&gt;platform groups&lt;/a&gt;, &lt;a href=../platformProg&gt;platform programs&lt;/a&gt;, &lt;a href=../procLev&gt;processing levels&lt;/a&gt;, &lt;a href=../product&gt;products&lt;/a&gt;, &lt;a href=../project&gt;projects&lt;/a&gt;, and &lt;a href=../sensor&gt;sensors&lt;/a&gt;. The use of a concept scheme allows easy navigation up and down the tree.&lt;/p&gt;&lt;h5&gt;SKOS Navigation Down the Concept Scheme&lt;/h5&gt;&lt;img src=conceptSchemeDown.svg /&gt;&lt;h5&gt;SKOS Navigation Up the Concept Scheme&lt;/h5&gt;&lt;img src=conceptSchemeUp.svg /&gt;&lt;p&gt;As well as being concepts the the concepts are also named individuals of the &lt;a href=../../../ontology/cci&gt;CCI Ontology&lt;/a&gt; classes.&lt;h5&gt;OWL Classes&lt;/h5&gt;&lt;img src=classes.svg /&gt;&lt;p&gt;&lt;/p&gt;</t>
+    <t>&lt;p&gt;The CCI concept schemes are used to define concepts within an element of a Directory Reference Scheme. There are currently eleven concept schemes defined: &lt;a href=../dataType&gt;data type&lt;/a&gt;, &lt;a href=..//ecv&gt;ecv&lt;/a&gt;, &lt;a href=../scheme/cci/freq&gt;frequency&lt;/a&gt;, &lt;a href=../org&gt;institutes&lt;/a&gt;, &lt;a href=../platform&gt;platforms&lt;/a&gt;, &lt;a href=../platformGrp&gt;platform groups&lt;/a&gt;, &lt;a href=../platformProg&gt;platform programs&lt;/a&gt;, &lt;a href=../procLev&gt;processing levels&lt;/a&gt;, &lt;a href=../product&gt;products&lt;/a&gt;, &lt;a href=../project&gt;projects&lt;/a&gt;, and &lt;a href=../sensor&gt;sensors&lt;/a&gt;. The use of a concept scheme allows easy navigation up and down the tree.&lt;/p&gt;&lt;p&gt;As well as being concepts, all of the concepts are also named individuals of the &lt;a href=../../../ontology/cci&gt;CCI Ontology&lt;/a&gt; classes.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF3300C-39A4-7B44-84E0-196A8940B2E9}">
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1759,7 +1759,7 @@
       <c r="AMF1" s="4"/>
       <c r="AMG1" s="4"/>
     </row>
-    <row r="2" spans="1:1021" ht="84">
+    <row r="2" spans="1:1021" ht="70">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1021" ht="84">
+    <row r="3" spans="1:1021" ht="70">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:1021" ht="84">
+    <row r="4" spans="1:1021" ht="70">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:1021" ht="84">
+    <row r="5" spans="1:1021" ht="70">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:1021" ht="84">
+    <row r="6" spans="1:1021" ht="70">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:1021" ht="84">
+    <row r="7" spans="1:1021" ht="70">
       <c r="A7" s="6" t="s">
         <v>39</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:1021" ht="84">
+    <row r="8" spans="1:1021" ht="70">
       <c r="A8" s="6" t="s">
         <v>42</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:1021" ht="84">
+    <row r="9" spans="1:1021" ht="70">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:1021" ht="84">
+    <row r="10" spans="1:1021" ht="70">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:1021" ht="84">
+    <row r="11" spans="1:1021" ht="70">
       <c r="A11" s="6" t="s">
         <v>57</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1021" ht="84">
+    <row r="12" spans="1:1021" ht="70">
       <c r="A12" s="6" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
update descriptions in cci-ontology and cc-shemes xlsx files
</commit_message>
<xml_diff>
--- a/data/cci/cci-schemes.xlsx
+++ b/data/cci/cci-schemes.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies/data/cci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5C0294F-2D38-1E46-8D8F-4B64F7BF2E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE62E0D-82E7-8B42-9443-B003BDBFA535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-71620" yWindow="-2440" windowWidth="30240" windowHeight="18880" xr2:uid="{B107F907-321D-DF43-80B1-3451B0C1D4B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -79,249 +79,6 @@
     <t>This concept scheme represents the ECVs used by the CCI project</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">&lt;p&gt;The CCI concept schemes are used to define concepts within an element of a Directory Reference Scheme. There are currently eight concept schemes defined: &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../dataType&gt;data type&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t>=..//ecv&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>ecv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t>=../scheme/cci/freq&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>frequency</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t>=../org&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>institutes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../platform&gt;platforms&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../procLev&gt;processing levels&lt;/a&gt;, &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../product&gt;products&lt;/a&gt;, and &lt;a </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>href</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=../sensor&gt;sensors&lt;/a&gt;. The use of a concept scheme allows easy navigation up and down the tree.&lt;/p&gt;&lt;h5&gt;SKOS Navigation Down the Concept Scheme&lt;/h5&gt;&lt;img </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=conceptSchemeDown.svg /&gt;&lt;h5&gt;SKOS Navigation Up the Concept Scheme&lt;/h5&gt;&lt;img </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t xml:space="preserve">=conceptSchemeUp.svg /&gt;&lt;p&gt;As well as being concepts the the concepts are also named individuals of the &lt;a href=../../../ontology/cci&gt;CCI Ontology&lt;/a&gt; classes.&lt;h5&gt;OWL Classes&lt;/h5&gt;&lt;img </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF313739"/>
-        <rFont val="Monospace"/>
-      </rPr>
-      <t>src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans1"/>
-      </rPr>
-      <t>=classes.svg /&gt;&lt;p&gt;&lt;/p&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>0.0.1</t>
   </si>
   <si>
@@ -434,6 +191,9 @@
   </si>
   <si>
     <t>This concept scheme represents the sensors used by the CCI project</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The CCI concept schemes are used to define concepts within an element of a Directory Reference Scheme. There are currently 10 concept schemes defined: &lt;a href=../dataType&gt;data type&lt;/a&gt;, &lt;a href=..//ecv&gt;ecv&lt;/a&gt;, &lt;a href=../scheme/cci/freq&gt;frequency&lt;/a&gt;, &lt;a href=../org&gt;institutes&lt;/a&gt;, &lt;a href=../platform&gt;platforms&lt;/a&gt;, &lt;a href=../platformGrp&gt;platform groups&lt;/a&gt;, &lt;a href=../platformProg&gt;platform programmes&lt;/a&gt;, &lt;a href=../procLev&gt;processing levels&lt;/a&gt;, &lt;a href=../product&gt;products&lt;/a&gt;,  and &lt;a href=../sensor&gt;sensors&lt;/a&gt;. The use of a concept scheme allows easy navigation up and down the tree.&lt;/p&gt;&lt;p&gt;As well as being concepts, all of the concepts are also named individuals of the &lt;a href=../../../ontology/cci&gt;CCI Ontology&lt;/a&gt; classes.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -443,7 +203,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -474,12 +234,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Liberation Sans1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF313739"/>
-      <name val="Monospace"/>
     </font>
     <font>
       <sz val="10"/>
@@ -555,7 +309,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -575,16 +329,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -925,13 +673,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF3300C-39A4-7B44-84E0-196A8940B2E9}">
-  <dimension ref="A1:XFD11"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="31" style="5" customWidth="1"/>
     <col min="2" max="3" width="31.6640625" style="5" customWidth="1"/>
@@ -1999,348 +1747,348 @@
       <c r="AMF1" s="4"/>
       <c r="AMG1" s="4"/>
     </row>
-    <row r="2" spans="1:1021" ht="70">
+    <row r="2" spans="1:1021" ht="56">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="6"/>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:1021" ht="56">
+      <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:1021" ht="70">
-      <c r="A3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8" t="s">
+    <row r="4" spans="1:1021" ht="56">
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="4" spans="1:1021" ht="70">
-      <c r="A4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8" t="s">
+    <row r="5" spans="1:1021" ht="56">
+      <c r="A5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L5" s="7"/>
+      <c r="M5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="6" t="s">
+      <c r="N5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="5" spans="1:1021" ht="70">
-      <c r="A5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+    <row r="6" spans="1:1021" ht="56">
+      <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="6" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L6" s="7"/>
+      <c r="M6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="6" spans="1:1021" ht="70">
-      <c r="A6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
+    <row r="7" spans="1:1021" ht="56">
+      <c r="A7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
+      <c r="J7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1021" ht="56">
+      <c r="A8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="6" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L8" s="7"/>
+      <c r="M8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="6" t="s">
+      <c r="N8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="7" spans="1:1021" ht="70">
-      <c r="A7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
+    <row r="9" spans="1:1021" ht="56">
+      <c r="A9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="6" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L9" s="7"/>
+      <c r="M9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="6" t="s">
+      <c r="N9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="8" spans="1:1021" ht="70">
-      <c r="A8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8" t="s">
+    <row r="10" spans="1:1021" ht="56">
+      <c r="A10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="6" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="L10" s="7"/>
+      <c r="M10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="6" t="s">
+      <c r="N10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="9" spans="1:1021" ht="70">
-      <c r="A9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
+    <row r="11" spans="1:1021" ht="56">
+      <c r="A11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="6" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="L11" s="7"/>
+      <c r="M11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="6" t="s">
+      <c r="N11" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1021" ht="70">
-      <c r="A10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1021" ht="70">
-      <c r="A11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>